<commit_message>
feat.Making OrderList, Send Ebook
</commit_message>
<xml_diff>
--- a/comments.xlsx
+++ b/comments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,68 +453,850 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>이레아 Irea</t>
+          <t>김지민</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>완벽하고 싶은마음이 커서 회피하고 싶은 마음 너무 저 같아서 공감이 가네요..ㅠㅠ 멀리서나마 응원하겠습니다..!!</t>
+          <t>한수빈 / yunyejun@example.org</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2023.6.18. 17:16</t>
+          <t>1991-08-17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>김늘보</t>
+          <t>양시우</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>이레아님 공감과 응원 정말 감사합니다!ㅠㅠㅠ</t>
+          <t>김서영 / shwang@example.net</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2023.6.18. 17:17</t>
+          <t>2006-07-30</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>마케터 뮤즈</t>
+          <t>이정호</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>할 건 많고 넘 힘들죠 ㅠ 번아웃 잘 관리하시구 힘내요!! 잘될거에요 🥹👍🏻</t>
+          <t>황영길 / jihyeonsug@example.org</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2023.6.18. 17:22</t>
+          <t>1970-06-20</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>김늘보</t>
+          <t>최도현</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>감사합니다ㅠㅠㅠ 힘드네요😢</t>
+          <t>허준호 / iminjun@example.com</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2023.6.18. 17:24</t>
+          <t>1987-11-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>김채원</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>김수진 / seongmingang@example.net</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2015-10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>김병철</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>이예지 / minjinho@example.org</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1981-04-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>이영수</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>김성현 / misug64@example.org</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1996-08-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>김영숙</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>권영숙 / cunja91@example.com</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2012-02-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>안예준</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>엄현주 / iminjun@example.org</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2005-04-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>김승현</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>황성민 / jeongsiggim@example.net</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1986-12-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>김예원</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>김영길 / guyeji@example.com</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1987-01-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>윤선영</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>박진호 / ti@example.org</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1976-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>김성현</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>윤상호 / ansunog@example.net</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2004-06-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>양민석</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>최지민 / junseocoe@example.net</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1999-12-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>백지현</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>김승민 / jieungim@example.net</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1987-06-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>이도현</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>김광수 / yeongjago@example.com</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>1994-09-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>황재현</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>김영호 / eunju62@example.org</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2018-09-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>곽민서</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>배성민 / idonghyeon@example.net</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1991-07-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>김춘자</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>김광수 / dmun@example.org</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1987-07-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>이우진</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>최승민 / rgim@example.com</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1981-10-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>문미숙</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>김은지 / jeongsuggim@example.org</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2000-05-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>김순옥</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>김옥순 / cgang@example.net</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2007-04-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>이민석</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>김아름 / yi@example.org</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>1996-06-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>이은지</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>문민지 / misug22@example.com</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2017-01-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>김정훈</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>박지은 / gyeongsug59@example.org</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>1977-03-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>심은영</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>이현숙 / minjunseo@example.com</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2015-07-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>심수진</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>이성수 / byeongceol43@example.org</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>1984-04-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>손영자</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>이은서 / jsong@example.com</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1993-10-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>김민재</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>한명숙 / mijeonggang@example.com</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>1992-10-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>이현정</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>김진호 / jiagim@example.org</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>1970-07-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>강주원</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>김민지 / coesumin@example.net</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2003-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>박정순</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>권진우 / sangceol41@example.org</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2022-05-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>김영식</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>송은서 / qjang@example.net</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1979-03-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>홍도윤</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>서지현 / johaeun@example.net</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2010-10-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>최미숙</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>오성수 / gimminjun@example.net</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2008-10-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>허진호</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>손상현 / gimhyeonjun@example.net</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>1994-01-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>박은서</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>노미경 / jihyean@example.org</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>1971-07-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>이현지</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>박정남 / bhong@example.com</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2021-06-07</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>배상훈</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>김재호 / seojun51@example.com</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2019-05-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>한성호</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>권정웅 / gweonjeongsu@example.net</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>1975-08-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>이영수</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>박상현 / bagyeonggil@example.org</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>1992-05-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>나현정</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>이지영 / sumini@example.net</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2011-05-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>강재호</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>최예준 / minji22@example.com</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>1993-09-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>김민지</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>류도윤 / ni@example.com</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2009-03-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>오재현</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>류하윤 / boram42@example.org</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>1995-04-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>양명숙</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>최민서 / mo@example.org</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>1993-02-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>김정호</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>서선영 / ui@example.com</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>1997-06-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>강병철</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>김미영 / sanghyeoni@example.net</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2006-02-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>정영자</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>박옥자 / seohyeon88@example.org</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>1999-11-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>박정식</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>최수민 / hwanggeonu@example.org</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2015-10-31</t>
         </is>
       </c>
     </row>

</xml_diff>